<commit_message>
Update for April metrics.
</commit_message>
<xml_diff>
--- a/Code/Failure_rate/2022/YTD_2022.xlsx
+++ b/Code/Failure_rate/2022/YTD_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\Failure_rate\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F692EDC9-A33B-43E1-BE97-FBC4EF2924A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF89544-0EAE-473F-B909-7726A10A191C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20550" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16635" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="1231">
   <si>
     <t>RMA ID</t>
   </si>
@@ -2901,6 +2901,819 @@
   </si>
   <si>
     <t>CONNECT 4" SQUARE BEVEL CT HSG 15W CLASSIC 120-277V D6E ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16912</t>
+  </si>
+  <si>
+    <t>RPB-01-15CS3-UNV-D6A-MOD1</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX 15W CS3 280mA 120-277V D6A-MOD=CSD 2CH BLACK ROCK</t>
+  </si>
+  <si>
+    <t>RMA16908</t>
+  </si>
+  <si>
+    <t>SP-285-02-RD-F</t>
+  </si>
+  <si>
+    <t>3" MINI BASIC EC ADPT REPLACEMENT KIT-ROUND FLANGED</t>
+  </si>
+  <si>
+    <t>RMA16907</t>
+  </si>
+  <si>
+    <t>LEM-213-00-40KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BASIC BEVELED STD CRI 4000K</t>
+  </si>
+  <si>
+    <t>RMA16906</t>
+  </si>
+  <si>
+    <t>M1RDF-07X4C-30KH-50-M0-WH-WH-RT-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRMD 7W 3000K 90 CRI 50° BEAM MICRO DIF LENS WHITE WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RPD-04-07X4C-UNV-D6E</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER LITTLEONES-4 FIXTURE MAX-7W X4C 700mA 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA16905</t>
+  </si>
+  <si>
+    <t>SP-359-1</t>
+  </si>
+  <si>
+    <t>REPLACEMENT CONTROLLER PLATE ASSY-MINI FTA CS AC166 NON ELDO</t>
+  </si>
+  <si>
+    <t>RMA16904</t>
+  </si>
+  <si>
+    <t>SP-317-0350-28</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NC HSG 9W 350mA 120V-277V  ELDO DMX 0.1%</t>
+  </si>
+  <si>
+    <t>RMA16903</t>
+  </si>
+  <si>
+    <t>LEM-293-00-35KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.1/2.2 36W 80CRI 3500K</t>
+  </si>
+  <si>
+    <t>RMA16902</t>
+  </si>
+  <si>
+    <t>SP-324-0350-3</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT DRIVER - REPLACEMENT MINI X FTA-0350mA 120V-277V DIML3-TR</t>
+  </si>
+  <si>
+    <t>RMA16901</t>
+  </si>
+  <si>
+    <t>B3RAL-25-S-BL-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI ROUND DL/ADJ TRML SOLITE LENS BLACK</t>
+  </si>
+  <si>
+    <t>C - REP ERROR</t>
+  </si>
+  <si>
+    <t>B3RAL-18CS1-6022KS-40-NC1-UNV-D28-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD ADJ TRML 18W COLOR SELECT 60-22K 80CRI 40° BEAM NC1 HSG 120-277V D28</t>
+  </si>
+  <si>
+    <t>RMA16900</t>
+  </si>
+  <si>
+    <t>USAI-4DLD1NM-TW1IV32A-RFK-00</t>
+  </si>
+  <si>
+    <t>RECESS 4.5 RD DL TRMD 32W COLOR SELECT 60-22K 80CRI 60°BEAM NCSM HSG 120-277V 0-10V 1% DIM</t>
+  </si>
+  <si>
+    <t>RMA16899</t>
+  </si>
+  <si>
+    <t>RMA16898</t>
+  </si>
+  <si>
+    <t>SP-172-0700-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED PENDANT CSD 32W 0700mA 120V-277V DIML6e EL-0-10</t>
+  </si>
+  <si>
+    <t>SP-250-1</t>
+  </si>
+  <si>
+    <t>REPLACEMENT CONTROLLER-COLOR SELECT 2.0/MINI/5.0 NC/NCSM/FT</t>
+  </si>
+  <si>
+    <t>RMA16897</t>
+  </si>
+  <si>
+    <t>RPC-01-16C3-120V-D3</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER BEVELED-1 FIXTURE MAX-16W C3 700mA 120V D3</t>
+  </si>
+  <si>
+    <t>RMA16896</t>
+  </si>
+  <si>
+    <t>RMA16895</t>
+  </si>
+  <si>
+    <t>B4RDF-32CS1-6022KS-60-NCSM-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD DL TRMD 32W COLOR SELECT 60-22K 80CRI 60° BEAM NCSM HSG 120-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16894</t>
+  </si>
+  <si>
+    <t>LEM-275-16-3022KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 WG2 16W 90CRI 3000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16893</t>
+  </si>
+  <si>
+    <t>MDG06-21H1-35KH-50-BG-BL-GL94-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 6 CELL 21W 3500K 90 CRI 50° BLACK SPECULAR-BLACK GL94 TRIM</t>
+  </si>
+  <si>
+    <t>RMA16892</t>
+  </si>
+  <si>
+    <t>A1-661-NC-01B</t>
+  </si>
+  <si>
+    <t>EM BATT ASM-IOTA STD AC164 4"NC</t>
+  </si>
+  <si>
+    <t>SP-317-1050-6E-EM</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NC HSG 24W 1050mA 120V-277V-ELDO 1% LIN DIM EM</t>
+  </si>
+  <si>
+    <t>RMA16891</t>
+  </si>
+  <si>
+    <t>RMA16890</t>
+  </si>
+  <si>
+    <t>SP-373-0900-28</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NCSM HSG E1 36W 900mA 120V-277V ELDO DMX 0.1%</t>
+  </si>
+  <si>
+    <t>RMA16889</t>
+  </si>
+  <si>
+    <t>RMA16888</t>
+  </si>
+  <si>
+    <t>A3-232-NC1-05</t>
+  </si>
+  <si>
+    <t>HSG MINI NC1-MINI-X</t>
+  </si>
+  <si>
+    <t>RMA16887</t>
+  </si>
+  <si>
+    <t>M1SDL-09X1M-30KH-35-M0-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO SQ DL TRML 9W 3000K 90 CRI 35° BEAM MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16886</t>
+  </si>
+  <si>
+    <t>RMA16885</t>
+  </si>
+  <si>
+    <t>LEM-402-A1-30H</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT - ZEPTO 90+CRI 3000K</t>
+  </si>
+  <si>
+    <t>RMA16884</t>
+  </si>
+  <si>
+    <t>B3RDF-15L2-35KS-50-NC1-UNV-D22-EM-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRMD 15W BASIC 35K 80CRI 50° BEAM NC1 HSG 120-277V D22 EM</t>
+  </si>
+  <si>
+    <t>B3RDF-15L2-35KS-50-NC1-UNV-D22-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRMD 15W BASIC 35K 80CRI 50° BEAM NC1 HSG 120-277V D22</t>
+  </si>
+  <si>
+    <t>RMA16883</t>
+  </si>
+  <si>
+    <t>AL20M</t>
+  </si>
+  <si>
+    <t>SIZE M-ACCESSORY LENS MICRODIFFUSION 20 X 20° BEAM</t>
+  </si>
+  <si>
+    <t>SV-X115-NC-UNV-D6E</t>
+  </si>
+  <si>
+    <t>SLIVERLED SQ/RND TRIMMED 15W NEW CONSTRUCTION HSG 120-277V-DIML6E</t>
+  </si>
+  <si>
+    <t>SS21-BL-X115-30KS-25-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>SLIVERLED SQ ADJ REGRESS BLCK BFFL X115 3000KS-25°DISTRIBUTION-SOLITE CLEAR LENS-WHITE TRM</t>
+  </si>
+  <si>
+    <t>RMA16882</t>
+  </si>
+  <si>
+    <t>RMA16881</t>
+  </si>
+  <si>
+    <t>RMA16880</t>
+  </si>
+  <si>
+    <t>SP-192-RJ</t>
+  </si>
+  <si>
+    <t>INTERFACE- DMX SIGNAL WRGB- RJ45</t>
+  </si>
+  <si>
+    <t>SP-175-0700-1M</t>
+  </si>
+  <si>
+    <t>DRIVER ASM BEVELED WRGB- 32W 350/350/350/700mA 120V-277V NC/IC/CP 8 BIT MANUAL ADDRESSING DMX DIM-EL</t>
+  </si>
+  <si>
+    <t>RMA16879</t>
+  </si>
+  <si>
+    <t>RMA16878</t>
+  </si>
+  <si>
+    <t>RMA16877</t>
+  </si>
+  <si>
+    <t>B4RDF-16WG2-3022KS-50-NC-UNV-D6E-EM-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD DL TRMD 16W WARM GLOW 30-22K 80CRI 50° BEAM NC HSG 120-277V ELDO 1% LIN DIM EM</t>
+  </si>
+  <si>
+    <t>RMA16876</t>
+  </si>
+  <si>
+    <t>P3RDF-15L2-30KS-M-WH-EC-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI PRIMARY ROUND DL TRMD 15W L2 30K 80CRI MEDIUM WHITE EC TRIM</t>
+  </si>
+  <si>
+    <t>RMA16875</t>
+  </si>
+  <si>
+    <t>BLRD5-16C3-35KH-50-S-WH-CC-UNV-D2</t>
+  </si>
+  <si>
+    <t>BEVELED BLOCK RD 16W 3500KH-50° DL-SOLITE LENS-WHITE-CONDUIT CUTOUTS 120-277V DIML2</t>
+  </si>
+  <si>
+    <t>RMA16874</t>
+  </si>
+  <si>
+    <t>RPC-01-12C3-UNV-D6E-EM5</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER BEVELED-1 FIXTURE MAX-12W C3 500mA 120-277V D6E-EM 5W</t>
+  </si>
+  <si>
+    <t>BLSD5-12C3-35KS-50-S-SC-PJ3-UNV-D6E</t>
+  </si>
+  <si>
+    <t>BEVELED BLOCK SQ 12W 3500KS-50° DL-SOLITE LENS-CONDUIT SILVER-PJ MOUNT 49"-95" 120-277V DIML6E</t>
+  </si>
+  <si>
+    <t>RMA16873</t>
+  </si>
+  <si>
+    <t>LED-203-40B</t>
+  </si>
+  <si>
+    <t>NANO LED CREE MTG2 4000K STD CRI</t>
+  </si>
+  <si>
+    <t>RMA16872</t>
+  </si>
+  <si>
+    <t>RMA16870</t>
+  </si>
+  <si>
+    <t>RMA16869</t>
+  </si>
+  <si>
+    <t>LEM-329-00-6022KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT LIGH ENGINE- (24) XD16 COLOR SELECT MINI CS2 STD CRI 6000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16868</t>
+  </si>
+  <si>
+    <t>SP-312-0500-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 FT HSG 12W 500mA 120V-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16867</t>
+  </si>
+  <si>
+    <t>RMA16866</t>
+  </si>
+  <si>
+    <t>RMA16865</t>
+  </si>
+  <si>
+    <t>SP-087-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-BEVELED 6" PENDANT-9W-350mA-120V-277V-DIML6E-EL</t>
+  </si>
+  <si>
+    <t>SP-087-0700-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-BEVELED 6" PENDANT-16W-700mA-120V-277V DIML6E-EL</t>
+  </si>
+  <si>
+    <t>RMA16864</t>
+  </si>
+  <si>
+    <t>RPD-01-15X1M-120V-D3</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER LITTLEONES-1 FIXTURE/DRIVER-15W X1M 350mA 120V D3</t>
+  </si>
+  <si>
+    <t>RPD-03-15X4C-120V-D3</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER LITTLEONES-3 FIXTURES/DRIVER-15W X4C 1300mA 120V D3</t>
+  </si>
+  <si>
+    <t>RMA16863</t>
+  </si>
+  <si>
+    <t>RMA16862</t>
+  </si>
+  <si>
+    <t>RMA16861</t>
+  </si>
+  <si>
+    <t>B3RDF-20X3-27KS-40-NC1-120V-D19-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRMD 20W CLASSIC 27K 80CRI 40° BEAM NC1 HSG 120V D19 PHASE 1% DIM</t>
+  </si>
+  <si>
+    <t>RMA16860</t>
+  </si>
+  <si>
+    <t>RMA16859</t>
+  </si>
+  <si>
+    <t>RMA16858</t>
+  </si>
+  <si>
+    <t>USAI-2CRNC-CXXIP15A-00</t>
+  </si>
+  <si>
+    <t>SAVANT/USAI CORE 2 CLASIC WHITE INTEGRAL 120V PHASE 15W NC HSG</t>
+  </si>
+  <si>
+    <t>RMA16857</t>
+  </si>
+  <si>
+    <t>RMA16856</t>
+  </si>
+  <si>
+    <t>USAI-4DL-LED-TW1XX-00</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-RECESS 4.5 TW1 16-32W 80CRI 6000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16855</t>
+  </si>
+  <si>
+    <t>SP-519-0700-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - BEVELED 2.2 CYLINDER CS1 32W 700mA 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA16854</t>
+  </si>
+  <si>
+    <t>RMA16853</t>
+  </si>
+  <si>
+    <t>RMA16851</t>
+  </si>
+  <si>
+    <t>SP-189-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT SLIVERLED 350mA-DIML6E-EL</t>
+  </si>
+  <si>
+    <t>RMA16850</t>
+  </si>
+  <si>
+    <t>RMA16848</t>
+  </si>
+  <si>
+    <t>RMA16847</t>
+  </si>
+  <si>
+    <t>SP-339-S-BL</t>
+  </si>
+  <si>
+    <t>TRIM REPLACEMENT BEVELED BLOCK SQ DL-SOLITE-BLACK</t>
+  </si>
+  <si>
+    <t>RMA16846</t>
+  </si>
+  <si>
+    <t>RMA16845</t>
+  </si>
+  <si>
+    <t>RMA16844</t>
+  </si>
+  <si>
+    <t>B3RAF-S-GR-GR-TRM-MLC</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL/ADJ TRMD 0°-40° TILT SOLITE LENS -GREY BEVEL-GREY FLAN-MILLWORK CONVERSION TRIM</t>
+  </si>
+  <si>
+    <t>RMA16843</t>
+  </si>
+  <si>
+    <t>M1SDF-09X1M-27KH-50-M0-WH-WH-RT-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO SQ DL TRMD 9W 2700K 90 CRI 50° BEAM MICRO DIF LENS WHITE WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16841</t>
+  </si>
+  <si>
+    <t>RMA16839</t>
+  </si>
+  <si>
+    <t>RMA16838</t>
+  </si>
+  <si>
+    <t>B4RCL-32WG2-3022KH-65-NCIC-120V-D3-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD COMFORT TRML 32W WARM GLOW 30-22K 90CRI 65° BEAM NCIC HSG 120V LUTRON 2-WIRE DIM</t>
+  </si>
+  <si>
+    <t>RMA16837</t>
+  </si>
+  <si>
+    <t>RMA16836</t>
+  </si>
+  <si>
+    <t>SAMPLE BAG BEVELED 2.2</t>
+  </si>
+  <si>
+    <t>RMA16835</t>
+  </si>
+  <si>
+    <t>SP-464-0350-22-EML</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-MINI BASIC-9W 350mA NC1/NCIC/NCCP HSG DIML22 EML</t>
+  </si>
+  <si>
+    <t>RMA16834</t>
+  </si>
+  <si>
+    <t>6331-B1-F-10</t>
+  </si>
+  <si>
+    <t>BEVELED 5.0 ROUND TRIMLESS ADJ 6" WHITE-FROSTED LENS</t>
+  </si>
+  <si>
+    <t>RMA16833</t>
+  </si>
+  <si>
+    <t>RMA16832</t>
+  </si>
+  <si>
+    <t>SP-318-1050-6E-MOD-PD-2111-1</t>
+  </si>
+  <si>
+    <t>RMA16831</t>
+  </si>
+  <si>
+    <t>B3RDL-18CS1-6022KS-65-FT-RM-HSG-MOD2</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRML 18W CLR SLCT 60-22K 80CRI 65°FT HSG REMOTE DRVR-MOD=CLR SLCT LESS LIGHT ENGI</t>
+  </si>
+  <si>
+    <t>RMA16830</t>
+  </si>
+  <si>
+    <t>RMA16829</t>
+  </si>
+  <si>
+    <t>RMA16828</t>
+  </si>
+  <si>
+    <t>RMA16827</t>
+  </si>
+  <si>
+    <t>RMA16826</t>
+  </si>
+  <si>
+    <t>RMA16825</t>
+  </si>
+  <si>
+    <t>RMA16824</t>
+  </si>
+  <si>
+    <t>B3SDL-20X3-30KS-55-FT-120V-D19-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ DL TRML 20W CLASSIC 30K 80CRI 55° BEAM FT HSG 120V D19 PHASE 1% DIM</t>
+  </si>
+  <si>
+    <t>B3SDL-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELEDMINI SQ DL/ADJ TRML SOLITE LENS WHITE</t>
+  </si>
+  <si>
+    <t>RMA16823</t>
+  </si>
+  <si>
+    <t>MWF12-41H1-35KS-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO WALL WASH FLANGE 12 CELL 41W 3500KS WHITE-WHITE-TRIM</t>
+  </si>
+  <si>
+    <t>RMA16822</t>
+  </si>
+  <si>
+    <t>MDG04-13H1-NCVS-UNV-D6E-GL95-HSG</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 4 CELL 13W NCVS UNV ELDOLED 0-10V 1% LIN GL95 HSG</t>
+  </si>
+  <si>
+    <t>RMA16821</t>
+  </si>
+  <si>
+    <t>RMA16820</t>
+  </si>
+  <si>
+    <t>SP-318-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NCSM HSG C3 9W 350mA 120V-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16819</t>
+  </si>
+  <si>
+    <t>RPD-01-09X1M-120V-D3</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER LITTLEONES-1 FIXTURE/DRIVER-9W X1M 225mA 120V D3</t>
+  </si>
+  <si>
+    <t>RMA16818</t>
+  </si>
+  <si>
+    <t>RMA16817</t>
+  </si>
+  <si>
+    <t>RMA16816</t>
+  </si>
+  <si>
+    <t>RMA16815</t>
+  </si>
+  <si>
+    <t>USAI-3DLD1NC-TW1IV18A-SPI-00</t>
+  </si>
+  <si>
+    <t>SAVANT/USAI RECESS 3 DNL SQR TRML  6000-2200KS TUNABLE WHITE  55° BEAM INTEGRAL 0-10V LOW VOLTAGE 18</t>
+  </si>
+  <si>
+    <t>RMA16814</t>
+  </si>
+  <si>
+    <t>SP-323-0350-2</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT MINI X FT/FTIC-0350mA 120V-277V DIML2-TR</t>
+  </si>
+  <si>
+    <t>RMA16813</t>
+  </si>
+  <si>
+    <t>LEM-307-00-27KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT PRIMARY HI CRI 2700K</t>
+  </si>
+  <si>
+    <t>RMA16812</t>
+  </si>
+  <si>
+    <t>RMA16811</t>
+  </si>
+  <si>
+    <t>RMA16810</t>
+  </si>
+  <si>
+    <t>RMA16809</t>
+  </si>
+  <si>
+    <t>M1SDF-07X4C-30KS-50-M0-BL-WH-RT-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO SQ DL TRMD 7W 3000K 80 CRI 50° BEAM MICRO DIF LENS BLACK WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16808</t>
+  </si>
+  <si>
+    <t>RMA16807</t>
+  </si>
+  <si>
+    <t>SP-120-1300-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 6" DL 80W 1300mA 120V-277V DIML6E-EL</t>
+  </si>
+  <si>
+    <t>RMA16806</t>
+  </si>
+  <si>
+    <t>RMA16805</t>
+  </si>
+  <si>
+    <t>B4RDF-16G1-35KS-50-NC-UNV-D6E-EM-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 BASIC RD DL TRMD 16W CLASSIC 35K 80CRI 50° BEAM NC HSG 120-277V ELDO 1% LIN DIM EM</t>
+  </si>
+  <si>
+    <t>B4RDF-16G1-35KS-50-NC-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 BASIC RD DL TRMD 16W CLASSIC 35K 80CRI 50° BEAM NC HSG 120-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16804</t>
+  </si>
+  <si>
+    <t>LEM-274-00-27KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT SLIVERLED HI CRI 2700K</t>
+  </si>
+  <si>
+    <t>RMA16803</t>
+  </si>
+  <si>
+    <t>RMA16802</t>
+  </si>
+  <si>
+    <t>RMA16801</t>
+  </si>
+  <si>
+    <t>RMA16800</t>
+  </si>
+  <si>
+    <t>RMA16799</t>
+  </si>
+  <si>
+    <t>RMA16797</t>
+  </si>
+  <si>
+    <t>RMA16796</t>
+  </si>
+  <si>
+    <t>RMA16795</t>
+  </si>
+  <si>
+    <t>SP-317-0700-PM01</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NC HSG 16W 700mA MOLEX 1% DIM</t>
+  </si>
+  <si>
+    <t>RMA16793</t>
+  </si>
+  <si>
+    <t>SP-125-0500-4-2</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT- NANOLED MULTI NC HSG 4 POS 20W 500mA-120V-277V-DIML2-TR</t>
+  </si>
+  <si>
+    <t>RMA16792</t>
+  </si>
+  <si>
+    <t>MWM04-13H1-30KH-BL-TRM</t>
+  </si>
+  <si>
+    <t>MICRO WALL WASH TRIMLESS/MILLWORK 4 CELL 13W 3000KH BLACK TRIM</t>
+  </si>
+  <si>
+    <t>SP-244-0350-19</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-MICRO NC 13W 350mA DIML19-HT</t>
+  </si>
+  <si>
+    <t>RMA16791</t>
+  </si>
+  <si>
+    <t>RMA16789</t>
+  </si>
+  <si>
+    <t>MDF08-27H1-30KS-50-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT FLANGE 8 CELL 27W 3000KS 50° WHITE-WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16788</t>
+  </si>
+  <si>
+    <t>MDG06-21H1-35KS-50-BL-BL-GLXX-TRM-MOD1</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 6 CELL 21W 3500K 80 CRI 50° BLACK-BLACK TRIM MOD=RULAN PG 4-12-52D</t>
+  </si>
+  <si>
+    <t>RMA16787</t>
+  </si>
+  <si>
+    <t>RPB-01-14M2-UNV-D2</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX-14W M2 350mA 120-277V D2</t>
+  </si>
+  <si>
+    <t>April</t>
   </si>
 </sst>
 </file>
@@ -3234,14 +4047,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F502"/>
+  <dimension ref="A1:F652"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J349" sqref="J349"/>
+      <pane ySplit="1" topLeftCell="A530" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F652" sqref="F652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -13278,6 +14094,3006 @@
       </c>
       <c r="F502" t="s">
         <v>660</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>960</v>
+      </c>
+      <c r="B503" t="s">
+        <v>961</v>
+      </c>
+      <c r="C503">
+        <v>8</v>
+      </c>
+      <c r="D503" t="s">
+        <v>962</v>
+      </c>
+      <c r="E503" t="s">
+        <v>16</v>
+      </c>
+      <c r="F503" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>963</v>
+      </c>
+      <c r="B504" t="s">
+        <v>964</v>
+      </c>
+      <c r="C504">
+        <v>8</v>
+      </c>
+      <c r="D504" t="s">
+        <v>965</v>
+      </c>
+      <c r="E504" t="s">
+        <v>9</v>
+      </c>
+      <c r="F504" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>966</v>
+      </c>
+      <c r="B505" t="s">
+        <v>967</v>
+      </c>
+      <c r="C505">
+        <v>4</v>
+      </c>
+      <c r="D505" t="s">
+        <v>968</v>
+      </c>
+      <c r="E505" t="s">
+        <v>16</v>
+      </c>
+      <c r="F505" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>969</v>
+      </c>
+      <c r="B506" t="s">
+        <v>970</v>
+      </c>
+      <c r="C506">
+        <v>2</v>
+      </c>
+      <c r="D506" t="s">
+        <v>971</v>
+      </c>
+      <c r="E506" t="s">
+        <v>16</v>
+      </c>
+      <c r="F506" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>969</v>
+      </c>
+      <c r="B507" t="s">
+        <v>972</v>
+      </c>
+      <c r="C507">
+        <v>5</v>
+      </c>
+      <c r="D507" t="s">
+        <v>973</v>
+      </c>
+      <c r="E507" t="s">
+        <v>16</v>
+      </c>
+      <c r="F507" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>974</v>
+      </c>
+      <c r="B508" t="s">
+        <v>975</v>
+      </c>
+      <c r="C508">
+        <v>1</v>
+      </c>
+      <c r="D508" t="s">
+        <v>976</v>
+      </c>
+      <c r="E508" t="s">
+        <v>16</v>
+      </c>
+      <c r="F508" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>977</v>
+      </c>
+      <c r="B509" t="s">
+        <v>978</v>
+      </c>
+      <c r="C509">
+        <v>1</v>
+      </c>
+      <c r="D509" t="s">
+        <v>979</v>
+      </c>
+      <c r="E509" t="s">
+        <v>16</v>
+      </c>
+      <c r="F509" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>980</v>
+      </c>
+      <c r="B510" t="s">
+        <v>981</v>
+      </c>
+      <c r="C510">
+        <v>1</v>
+      </c>
+      <c r="D510" t="s">
+        <v>982</v>
+      </c>
+      <c r="E510" t="s">
+        <v>16</v>
+      </c>
+      <c r="F510" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>983</v>
+      </c>
+      <c r="B511" t="s">
+        <v>984</v>
+      </c>
+      <c r="C511">
+        <v>1</v>
+      </c>
+      <c r="D511" t="s">
+        <v>985</v>
+      </c>
+      <c r="E511" t="s">
+        <v>16</v>
+      </c>
+      <c r="F511" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>986</v>
+      </c>
+      <c r="B512" t="s">
+        <v>987</v>
+      </c>
+      <c r="C512">
+        <v>8</v>
+      </c>
+      <c r="D512" t="s">
+        <v>988</v>
+      </c>
+      <c r="E512" t="s">
+        <v>989</v>
+      </c>
+      <c r="F512" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>986</v>
+      </c>
+      <c r="B513" t="s">
+        <v>987</v>
+      </c>
+      <c r="C513">
+        <v>7</v>
+      </c>
+      <c r="D513" t="s">
+        <v>988</v>
+      </c>
+      <c r="E513" t="s">
+        <v>989</v>
+      </c>
+      <c r="F513" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>986</v>
+      </c>
+      <c r="B514" t="s">
+        <v>990</v>
+      </c>
+      <c r="C514">
+        <v>7</v>
+      </c>
+      <c r="D514" t="s">
+        <v>991</v>
+      </c>
+      <c r="E514" t="s">
+        <v>989</v>
+      </c>
+      <c r="F514" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>986</v>
+      </c>
+      <c r="B515" t="s">
+        <v>343</v>
+      </c>
+      <c r="C515">
+        <v>8</v>
+      </c>
+      <c r="D515" t="s">
+        <v>344</v>
+      </c>
+      <c r="E515" t="s">
+        <v>989</v>
+      </c>
+      <c r="F515" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>986</v>
+      </c>
+      <c r="B516" t="s">
+        <v>990</v>
+      </c>
+      <c r="C516">
+        <v>8</v>
+      </c>
+      <c r="D516" t="s">
+        <v>991</v>
+      </c>
+      <c r="E516" t="s">
+        <v>989</v>
+      </c>
+      <c r="F516" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>986</v>
+      </c>
+      <c r="B517" t="s">
+        <v>343</v>
+      </c>
+      <c r="C517">
+        <v>7</v>
+      </c>
+      <c r="D517" t="s">
+        <v>344</v>
+      </c>
+      <c r="E517" t="s">
+        <v>989</v>
+      </c>
+      <c r="F517" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>992</v>
+      </c>
+      <c r="B518" t="s">
+        <v>993</v>
+      </c>
+      <c r="C518">
+        <v>2</v>
+      </c>
+      <c r="D518" t="s">
+        <v>994</v>
+      </c>
+      <c r="E518" t="s">
+        <v>16</v>
+      </c>
+      <c r="F518" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>995</v>
+      </c>
+      <c r="B519" t="s">
+        <v>240</v>
+      </c>
+      <c r="C519">
+        <v>1</v>
+      </c>
+      <c r="D519" t="s">
+        <v>241</v>
+      </c>
+      <c r="E519" t="s">
+        <v>16</v>
+      </c>
+      <c r="F519" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>996</v>
+      </c>
+      <c r="B520" t="s">
+        <v>997</v>
+      </c>
+      <c r="C520">
+        <v>2</v>
+      </c>
+      <c r="D520" t="s">
+        <v>998</v>
+      </c>
+      <c r="E520" t="s">
+        <v>16</v>
+      </c>
+      <c r="F520" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>996</v>
+      </c>
+      <c r="B521" t="s">
+        <v>999</v>
+      </c>
+      <c r="C521">
+        <v>2</v>
+      </c>
+      <c r="D521" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E521" t="s">
+        <v>16</v>
+      </c>
+      <c r="F521" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C522">
+        <v>4</v>
+      </c>
+      <c r="D522" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E522" t="s">
+        <v>16</v>
+      </c>
+      <c r="F522" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B523" t="s">
+        <v>462</v>
+      </c>
+      <c r="C523">
+        <v>1</v>
+      </c>
+      <c r="D523" t="s">
+        <v>463</v>
+      </c>
+      <c r="E523" t="s">
+        <v>16</v>
+      </c>
+      <c r="F523" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B524" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C524">
+        <v>1</v>
+      </c>
+      <c r="D524" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E524" t="s">
+        <v>16</v>
+      </c>
+      <c r="F524" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B525" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C525">
+        <v>6</v>
+      </c>
+      <c r="D525" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E525" t="s">
+        <v>16</v>
+      </c>
+      <c r="F525" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B526" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C526">
+        <v>2</v>
+      </c>
+      <c r="D526" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E526" t="s">
+        <v>16</v>
+      </c>
+      <c r="F526" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B527" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C527">
+        <v>1</v>
+      </c>
+      <c r="D527" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E527" t="s">
+        <v>16</v>
+      </c>
+      <c r="F527" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B528" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C528">
+        <v>1</v>
+      </c>
+      <c r="D528" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E528" t="s">
+        <v>16</v>
+      </c>
+      <c r="F528" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B529" t="s">
+        <v>26</v>
+      </c>
+      <c r="C529">
+        <v>1</v>
+      </c>
+      <c r="D529" t="s">
+        <v>27</v>
+      </c>
+      <c r="E529" t="s">
+        <v>9</v>
+      </c>
+      <c r="F529" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C530">
+        <v>1</v>
+      </c>
+      <c r="D530" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E530" t="s">
+        <v>16</v>
+      </c>
+      <c r="F530" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B531" t="s">
+        <v>203</v>
+      </c>
+      <c r="C531">
+        <v>2</v>
+      </c>
+      <c r="D531" t="s">
+        <v>204</v>
+      </c>
+      <c r="E531" t="s">
+        <v>16</v>
+      </c>
+      <c r="F531" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C532">
+        <v>1</v>
+      </c>
+      <c r="D532" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E532" t="s">
+        <v>324</v>
+      </c>
+      <c r="F532" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B533" t="s">
+        <v>300</v>
+      </c>
+      <c r="C533">
+        <v>1</v>
+      </c>
+      <c r="D533" t="s">
+        <v>301</v>
+      </c>
+      <c r="E533" t="s">
+        <v>16</v>
+      </c>
+      <c r="F533" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B534" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C534">
+        <v>1</v>
+      </c>
+      <c r="D534" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E534" t="s">
+        <v>16</v>
+      </c>
+      <c r="F534" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B535" t="s">
+        <v>137</v>
+      </c>
+      <c r="C535">
+        <v>3</v>
+      </c>
+      <c r="D535" t="s">
+        <v>138</v>
+      </c>
+      <c r="E535" t="s">
+        <v>16</v>
+      </c>
+      <c r="F535" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C536">
+        <v>5</v>
+      </c>
+      <c r="D536" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E536" t="s">
+        <v>16</v>
+      </c>
+      <c r="F536" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C537">
+        <v>2</v>
+      </c>
+      <c r="D537" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E537" t="s">
+        <v>9</v>
+      </c>
+      <c r="F537" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C538">
+        <v>6</v>
+      </c>
+      <c r="D538" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E538" t="s">
+        <v>9</v>
+      </c>
+      <c r="F538" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C539">
+        <v>16</v>
+      </c>
+      <c r="D539" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E539" t="s">
+        <v>127</v>
+      </c>
+      <c r="F539" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C540">
+        <v>16</v>
+      </c>
+      <c r="D540" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E540" t="s">
+        <v>127</v>
+      </c>
+      <c r="F540" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B541" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C541">
+        <v>16</v>
+      </c>
+      <c r="D541" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E541" t="s">
+        <v>127</v>
+      </c>
+      <c r="F541" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B542" t="s">
+        <v>134</v>
+      </c>
+      <c r="C542">
+        <v>6</v>
+      </c>
+      <c r="D542" t="s">
+        <v>135</v>
+      </c>
+      <c r="E542" t="s">
+        <v>16</v>
+      </c>
+      <c r="F542" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B543" t="s">
+        <v>688</v>
+      </c>
+      <c r="C543">
+        <v>3</v>
+      </c>
+      <c r="D543" t="s">
+        <v>689</v>
+      </c>
+      <c r="E543" t="s">
+        <v>9</v>
+      </c>
+      <c r="F543" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B544" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C544">
+        <v>4</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E544" t="s">
+        <v>16</v>
+      </c>
+      <c r="F544" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B545" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C545">
+        <v>4</v>
+      </c>
+      <c r="D545" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E545" t="s">
+        <v>16</v>
+      </c>
+      <c r="F545" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B546" t="s">
+        <v>116</v>
+      </c>
+      <c r="C546">
+        <v>4</v>
+      </c>
+      <c r="D546" t="s">
+        <v>117</v>
+      </c>
+      <c r="E546" t="s">
+        <v>16</v>
+      </c>
+      <c r="F546" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B547" t="s">
+        <v>701</v>
+      </c>
+      <c r="C547">
+        <v>1</v>
+      </c>
+      <c r="D547" t="s">
+        <v>702</v>
+      </c>
+      <c r="E547" t="s">
+        <v>16</v>
+      </c>
+      <c r="F547" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B548" t="s">
+        <v>517</v>
+      </c>
+      <c r="C548">
+        <v>1</v>
+      </c>
+      <c r="D548" t="s">
+        <v>518</v>
+      </c>
+      <c r="E548" t="s">
+        <v>16</v>
+      </c>
+      <c r="F548" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B549" t="s">
+        <v>52</v>
+      </c>
+      <c r="C549">
+        <v>2</v>
+      </c>
+      <c r="D549" t="s">
+        <v>53</v>
+      </c>
+      <c r="E549" t="s">
+        <v>16</v>
+      </c>
+      <c r="F549" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C550">
+        <v>1</v>
+      </c>
+      <c r="D550" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E550" t="s">
+        <v>163</v>
+      </c>
+      <c r="F550" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C551">
+        <v>2</v>
+      </c>
+      <c r="D551" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E551" t="s">
+        <v>9</v>
+      </c>
+      <c r="F551" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C552">
+        <v>1</v>
+      </c>
+      <c r="D552" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E552" t="s">
+        <v>324</v>
+      </c>
+      <c r="F552" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C553">
+        <v>2</v>
+      </c>
+      <c r="D553" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E553" t="s">
+        <v>9</v>
+      </c>
+      <c r="F553" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C554">
+        <v>2</v>
+      </c>
+      <c r="D554" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E554" t="s">
+        <v>9</v>
+      </c>
+      <c r="F554" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C555">
+        <v>129</v>
+      </c>
+      <c r="D555" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E555" t="s">
+        <v>16</v>
+      </c>
+      <c r="F555" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B556" t="s">
+        <v>701</v>
+      </c>
+      <c r="C556">
+        <v>3</v>
+      </c>
+      <c r="D556" t="s">
+        <v>702</v>
+      </c>
+      <c r="E556" t="s">
+        <v>127</v>
+      </c>
+      <c r="F556" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C557">
+        <v>1</v>
+      </c>
+      <c r="D557" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E557" t="s">
+        <v>16</v>
+      </c>
+      <c r="F557" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C558">
+        <v>3</v>
+      </c>
+      <c r="D558" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E558" t="s">
+        <v>16</v>
+      </c>
+      <c r="F558" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B559" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C559">
+        <v>2</v>
+      </c>
+      <c r="D559" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E559" t="s">
+        <v>16</v>
+      </c>
+      <c r="F559" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B560" t="s">
+        <v>167</v>
+      </c>
+      <c r="C560">
+        <v>15</v>
+      </c>
+      <c r="D560" t="s">
+        <v>168</v>
+      </c>
+      <c r="E560" t="s">
+        <v>16</v>
+      </c>
+      <c r="F560" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B561" t="s">
+        <v>621</v>
+      </c>
+      <c r="C561">
+        <v>1</v>
+      </c>
+      <c r="D561" t="s">
+        <v>622</v>
+      </c>
+      <c r="E561" t="s">
+        <v>16</v>
+      </c>
+      <c r="F561" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C562">
+        <v>1</v>
+      </c>
+      <c r="D562" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E562" t="s">
+        <v>9</v>
+      </c>
+      <c r="F562" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B563" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C563">
+        <v>1</v>
+      </c>
+      <c r="D563" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E563" t="s">
+        <v>9</v>
+      </c>
+      <c r="F563" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B564" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C564">
+        <v>1</v>
+      </c>
+      <c r="D564" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E564" t="s">
+        <v>989</v>
+      </c>
+      <c r="F564" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B565" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C565">
+        <v>10</v>
+      </c>
+      <c r="D565" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E565" t="s">
+        <v>989</v>
+      </c>
+      <c r="F565" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B566" t="s">
+        <v>610</v>
+      </c>
+      <c r="C566">
+        <v>1</v>
+      </c>
+      <c r="D566" t="s">
+        <v>611</v>
+      </c>
+      <c r="E566" t="s">
+        <v>9</v>
+      </c>
+      <c r="F566" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B567" t="s">
+        <v>501</v>
+      </c>
+      <c r="C567">
+        <v>1</v>
+      </c>
+      <c r="D567" t="s">
+        <v>502</v>
+      </c>
+      <c r="E567" t="s">
+        <v>16</v>
+      </c>
+      <c r="F567" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B568" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C568">
+        <v>1</v>
+      </c>
+      <c r="D568" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E568" t="s">
+        <v>9</v>
+      </c>
+      <c r="F568" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B569" t="s">
+        <v>424</v>
+      </c>
+      <c r="C569">
+        <v>2</v>
+      </c>
+      <c r="D569" t="s">
+        <v>425</v>
+      </c>
+      <c r="E569" t="s">
+        <v>16</v>
+      </c>
+      <c r="F569" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B570" t="s">
+        <v>406</v>
+      </c>
+      <c r="C570">
+        <v>2</v>
+      </c>
+      <c r="D570" t="s">
+        <v>407</v>
+      </c>
+      <c r="E570" t="s">
+        <v>16</v>
+      </c>
+      <c r="F570" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B571" t="s">
+        <v>701</v>
+      </c>
+      <c r="C571">
+        <v>1</v>
+      </c>
+      <c r="D571" t="s">
+        <v>702</v>
+      </c>
+      <c r="E571" t="s">
+        <v>16</v>
+      </c>
+      <c r="F571" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B572" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C572">
+        <v>1</v>
+      </c>
+      <c r="D572" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E572" t="s">
+        <v>9</v>
+      </c>
+      <c r="F572" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B573" t="s">
+        <v>876</v>
+      </c>
+      <c r="C573">
+        <v>1</v>
+      </c>
+      <c r="D573" t="s">
+        <v>877</v>
+      </c>
+      <c r="E573" t="s">
+        <v>16</v>
+      </c>
+      <c r="F573" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B574" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C574">
+        <v>6</v>
+      </c>
+      <c r="D574" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E574" t="s">
+        <v>16</v>
+      </c>
+      <c r="F574" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B575" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C575">
+        <v>3</v>
+      </c>
+      <c r="D575" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E575" t="s">
+        <v>16</v>
+      </c>
+      <c r="F575" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B576" t="s">
+        <v>343</v>
+      </c>
+      <c r="C576">
+        <v>80</v>
+      </c>
+      <c r="D576" t="s">
+        <v>344</v>
+      </c>
+      <c r="E576" t="s">
+        <v>9</v>
+      </c>
+      <c r="F576" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B577" t="s">
+        <v>532</v>
+      </c>
+      <c r="C577">
+        <v>28</v>
+      </c>
+      <c r="D577" t="s">
+        <v>533</v>
+      </c>
+      <c r="E577" t="s">
+        <v>9</v>
+      </c>
+      <c r="F577" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C578">
+        <v>2</v>
+      </c>
+      <c r="D578" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E578" t="s">
+        <v>16</v>
+      </c>
+      <c r="F578" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B579" t="s">
+        <v>343</v>
+      </c>
+      <c r="C579">
+        <v>60</v>
+      </c>
+      <c r="D579" t="s">
+        <v>344</v>
+      </c>
+      <c r="E579" t="s">
+        <v>9</v>
+      </c>
+      <c r="F579" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B580" t="s">
+        <v>630</v>
+      </c>
+      <c r="C580">
+        <v>10</v>
+      </c>
+      <c r="D580" t="s">
+        <v>631</v>
+      </c>
+      <c r="E580" t="s">
+        <v>16</v>
+      </c>
+      <c r="F580" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C581">
+        <v>1</v>
+      </c>
+      <c r="D581" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E581" t="s">
+        <v>127</v>
+      </c>
+      <c r="F581" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B582" t="s">
+        <v>145</v>
+      </c>
+      <c r="C582">
+        <v>1</v>
+      </c>
+      <c r="D582" t="s">
+        <v>146</v>
+      </c>
+      <c r="E582" t="s">
+        <v>16</v>
+      </c>
+      <c r="F582" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B583" t="s">
+        <v>170</v>
+      </c>
+      <c r="C583">
+        <v>1</v>
+      </c>
+      <c r="D583" t="s">
+        <v>171</v>
+      </c>
+      <c r="E583" t="s">
+        <v>16</v>
+      </c>
+      <c r="F583" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C584">
+        <v>8</v>
+      </c>
+      <c r="D584" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E584" t="s">
+        <v>9</v>
+      </c>
+      <c r="F584" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B585" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C585">
+        <v>1</v>
+      </c>
+      <c r="D585" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E585" t="s">
+        <v>16</v>
+      </c>
+      <c r="F585" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B586" t="s">
+        <v>725</v>
+      </c>
+      <c r="C586">
+        <v>5</v>
+      </c>
+      <c r="D586" t="s">
+        <v>726</v>
+      </c>
+      <c r="E586" t="s">
+        <v>16</v>
+      </c>
+      <c r="F586" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B587" t="s">
+        <v>277</v>
+      </c>
+      <c r="C587">
+        <v>1</v>
+      </c>
+      <c r="D587" t="s">
+        <v>278</v>
+      </c>
+      <c r="E587" t="s">
+        <v>16</v>
+      </c>
+      <c r="F587" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B588" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C588">
+        <v>8</v>
+      </c>
+      <c r="D588" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E588" t="s">
+        <v>127</v>
+      </c>
+      <c r="F588" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B589" t="s">
+        <v>517</v>
+      </c>
+      <c r="C589">
+        <v>4</v>
+      </c>
+      <c r="D589" t="s">
+        <v>518</v>
+      </c>
+      <c r="E589" t="s">
+        <v>16</v>
+      </c>
+      <c r="F589" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B590" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C590">
+        <v>1</v>
+      </c>
+      <c r="D590" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E590" t="s">
+        <v>127</v>
+      </c>
+      <c r="F590" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B591" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C591">
+        <v>1</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E591" t="s">
+        <v>16</v>
+      </c>
+      <c r="F591" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B592" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C592">
+        <v>54</v>
+      </c>
+      <c r="D592" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E592" t="s">
+        <v>9</v>
+      </c>
+      <c r="F592" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B593" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C593">
+        <v>1</v>
+      </c>
+      <c r="D593" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E593" t="s">
+        <v>9</v>
+      </c>
+      <c r="F593" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B594" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C594">
+        <v>3</v>
+      </c>
+      <c r="D594" t="s">
+        <v>735</v>
+      </c>
+      <c r="E594" t="s">
+        <v>16</v>
+      </c>
+      <c r="F594" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B595" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C595">
+        <v>3</v>
+      </c>
+      <c r="D595" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E595" t="s">
+        <v>9</v>
+      </c>
+      <c r="F595" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B596" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C596">
+        <v>1</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E596" t="s">
+        <v>16</v>
+      </c>
+      <c r="F596" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B597" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C597">
+        <v>1</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E597" t="s">
+        <v>16</v>
+      </c>
+      <c r="F597" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B598" t="s">
+        <v>179</v>
+      </c>
+      <c r="C598">
+        <v>2</v>
+      </c>
+      <c r="D598" t="s">
+        <v>180</v>
+      </c>
+      <c r="E598" t="s">
+        <v>16</v>
+      </c>
+      <c r="F598" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B599" t="s">
+        <v>85</v>
+      </c>
+      <c r="C599">
+        <v>1</v>
+      </c>
+      <c r="D599" t="s">
+        <v>86</v>
+      </c>
+      <c r="E599" t="s">
+        <v>16</v>
+      </c>
+      <c r="F599" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B600" t="s">
+        <v>87</v>
+      </c>
+      <c r="C600">
+        <v>1</v>
+      </c>
+      <c r="D600" t="s">
+        <v>88</v>
+      </c>
+      <c r="E600" t="s">
+        <v>16</v>
+      </c>
+      <c r="F600" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B601" t="s">
+        <v>87</v>
+      </c>
+      <c r="C601">
+        <v>2</v>
+      </c>
+      <c r="D601" t="s">
+        <v>88</v>
+      </c>
+      <c r="E601" t="s">
+        <v>16</v>
+      </c>
+      <c r="F601" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B602" t="s">
+        <v>273</v>
+      </c>
+      <c r="C602">
+        <v>1</v>
+      </c>
+      <c r="D602" t="s">
+        <v>274</v>
+      </c>
+      <c r="E602" t="s">
+        <v>16</v>
+      </c>
+      <c r="F602" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B603" t="s">
+        <v>49</v>
+      </c>
+      <c r="C603">
+        <v>1</v>
+      </c>
+      <c r="D603" t="s">
+        <v>50</v>
+      </c>
+      <c r="E603" t="s">
+        <v>16</v>
+      </c>
+      <c r="F603" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B604" t="s">
+        <v>151</v>
+      </c>
+      <c r="C604">
+        <v>6</v>
+      </c>
+      <c r="D604" t="s">
+        <v>152</v>
+      </c>
+      <c r="E604" t="s">
+        <v>16</v>
+      </c>
+      <c r="F604" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C605">
+        <v>2</v>
+      </c>
+      <c r="D605" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E605" t="s">
+        <v>9</v>
+      </c>
+      <c r="F605" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B606" t="s">
+        <v>343</v>
+      </c>
+      <c r="C606">
+        <v>2</v>
+      </c>
+      <c r="D606" t="s">
+        <v>344</v>
+      </c>
+      <c r="E606" t="s">
+        <v>9</v>
+      </c>
+      <c r="F606" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B607" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C607">
+        <v>2</v>
+      </c>
+      <c r="D607" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E607" t="s">
+        <v>9</v>
+      </c>
+      <c r="F607" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B608" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C608">
+        <v>13</v>
+      </c>
+      <c r="D608" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E608" t="s">
+        <v>16</v>
+      </c>
+      <c r="F608" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B609" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C609">
+        <v>1</v>
+      </c>
+      <c r="D609" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E609" t="s">
+        <v>9</v>
+      </c>
+      <c r="F609" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B610" t="s">
+        <v>55</v>
+      </c>
+      <c r="C610">
+        <v>2</v>
+      </c>
+      <c r="D610" t="s">
+        <v>56</v>
+      </c>
+      <c r="E610" t="s">
+        <v>16</v>
+      </c>
+      <c r="F610" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B611" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C611">
+        <v>1</v>
+      </c>
+      <c r="D611" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E611" t="s">
+        <v>16</v>
+      </c>
+      <c r="F611" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B612" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C612">
+        <v>1</v>
+      </c>
+      <c r="D612" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E612" t="s">
+        <v>16</v>
+      </c>
+      <c r="F612" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B613" t="s">
+        <v>129</v>
+      </c>
+      <c r="C613">
+        <v>3</v>
+      </c>
+      <c r="D613" t="s">
+        <v>130</v>
+      </c>
+      <c r="E613" t="s">
+        <v>16</v>
+      </c>
+      <c r="F613" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B614" t="s">
+        <v>33</v>
+      </c>
+      <c r="C614">
+        <v>3</v>
+      </c>
+      <c r="D614" t="s">
+        <v>34</v>
+      </c>
+      <c r="E614" t="s">
+        <v>16</v>
+      </c>
+      <c r="F614" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B615" t="s">
+        <v>675</v>
+      </c>
+      <c r="C615">
+        <v>2</v>
+      </c>
+      <c r="D615" t="s">
+        <v>676</v>
+      </c>
+      <c r="E615" t="s">
+        <v>16</v>
+      </c>
+      <c r="F615" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B616" t="s">
+        <v>734</v>
+      </c>
+      <c r="C616">
+        <v>1</v>
+      </c>
+      <c r="D616" t="s">
+        <v>735</v>
+      </c>
+      <c r="E616" t="s">
+        <v>16</v>
+      </c>
+      <c r="F616" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B617" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C617">
+        <v>1</v>
+      </c>
+      <c r="D617" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E617" t="s">
+        <v>16</v>
+      </c>
+      <c r="F617" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B618" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C618">
+        <v>4</v>
+      </c>
+      <c r="D618" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E618" t="s">
+        <v>163</v>
+      </c>
+      <c r="F618" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B619" t="s">
+        <v>145</v>
+      </c>
+      <c r="C619">
+        <v>1</v>
+      </c>
+      <c r="D619" t="s">
+        <v>146</v>
+      </c>
+      <c r="E619" t="s">
+        <v>16</v>
+      </c>
+      <c r="F619" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B620" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C620">
+        <v>1</v>
+      </c>
+      <c r="D620" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E620" t="s">
+        <v>16</v>
+      </c>
+      <c r="F620" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B621" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C621">
+        <v>1</v>
+      </c>
+      <c r="D621" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E621" t="s">
+        <v>16</v>
+      </c>
+      <c r="F621" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B622" t="s">
+        <v>70</v>
+      </c>
+      <c r="C622">
+        <v>1</v>
+      </c>
+      <c r="D622" t="s">
+        <v>71</v>
+      </c>
+      <c r="E622" t="s">
+        <v>16</v>
+      </c>
+      <c r="F622" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B623" t="s">
+        <v>725</v>
+      </c>
+      <c r="C623">
+        <v>1</v>
+      </c>
+      <c r="D623" t="s">
+        <v>726</v>
+      </c>
+      <c r="E623" t="s">
+        <v>16</v>
+      </c>
+      <c r="F623" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B624" t="s">
+        <v>489</v>
+      </c>
+      <c r="C624">
+        <v>1</v>
+      </c>
+      <c r="D624" t="s">
+        <v>490</v>
+      </c>
+      <c r="E624" t="s">
+        <v>16</v>
+      </c>
+      <c r="F624" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B625" t="s">
+        <v>691</v>
+      </c>
+      <c r="C625">
+        <v>1</v>
+      </c>
+      <c r="D625" t="s">
+        <v>692</v>
+      </c>
+      <c r="E625" t="s">
+        <v>16</v>
+      </c>
+      <c r="F625" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B626" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C626">
+        <v>2</v>
+      </c>
+      <c r="D626" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E626" t="s">
+        <v>16</v>
+      </c>
+      <c r="F626" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B627" t="s">
+        <v>148</v>
+      </c>
+      <c r="C627">
+        <v>60</v>
+      </c>
+      <c r="D627" t="s">
+        <v>149</v>
+      </c>
+      <c r="E627" t="s">
+        <v>127</v>
+      </c>
+      <c r="F627" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C628">
+        <v>3</v>
+      </c>
+      <c r="D628" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E628" t="s">
+        <v>9</v>
+      </c>
+      <c r="F628" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B629" t="s">
+        <v>145</v>
+      </c>
+      <c r="C629">
+        <v>1</v>
+      </c>
+      <c r="D629" t="s">
+        <v>146</v>
+      </c>
+      <c r="E629" t="s">
+        <v>16</v>
+      </c>
+      <c r="F629" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="630" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B630" t="s">
+        <v>148</v>
+      </c>
+      <c r="C630">
+        <v>6</v>
+      </c>
+      <c r="D630" t="s">
+        <v>149</v>
+      </c>
+      <c r="E630" t="s">
+        <v>9</v>
+      </c>
+      <c r="F630" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B631" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C631">
+        <v>6</v>
+      </c>
+      <c r="D631" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E631" t="s">
+        <v>9</v>
+      </c>
+      <c r="F631" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C632">
+        <v>94</v>
+      </c>
+      <c r="D632" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E632" t="s">
+        <v>9</v>
+      </c>
+      <c r="F632" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B633" t="s">
+        <v>148</v>
+      </c>
+      <c r="C633">
+        <v>94</v>
+      </c>
+      <c r="D633" t="s">
+        <v>149</v>
+      </c>
+      <c r="E633" t="s">
+        <v>9</v>
+      </c>
+      <c r="F633" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B634" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C634">
+        <v>1</v>
+      </c>
+      <c r="D634" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E634" t="s">
+        <v>16</v>
+      </c>
+      <c r="F634" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B635" t="s">
+        <v>273</v>
+      </c>
+      <c r="C635">
+        <v>10</v>
+      </c>
+      <c r="D635" t="s">
+        <v>274</v>
+      </c>
+      <c r="E635" t="s">
+        <v>16</v>
+      </c>
+      <c r="F635" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B636" t="s">
+        <v>87</v>
+      </c>
+      <c r="C636">
+        <v>26</v>
+      </c>
+      <c r="D636" t="s">
+        <v>88</v>
+      </c>
+      <c r="E636" t="s">
+        <v>16</v>
+      </c>
+      <c r="F636" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B637" t="s">
+        <v>73</v>
+      </c>
+      <c r="C637">
+        <v>1</v>
+      </c>
+      <c r="D637" t="s">
+        <v>74</v>
+      </c>
+      <c r="E637" t="s">
+        <v>16</v>
+      </c>
+      <c r="F637" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B638" t="s">
+        <v>179</v>
+      </c>
+      <c r="C638">
+        <v>12</v>
+      </c>
+      <c r="D638" t="s">
+        <v>180</v>
+      </c>
+      <c r="E638" t="s">
+        <v>16</v>
+      </c>
+      <c r="F638" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B639" t="s">
+        <v>49</v>
+      </c>
+      <c r="C639">
+        <v>1</v>
+      </c>
+      <c r="D639" t="s">
+        <v>50</v>
+      </c>
+      <c r="E639" t="s">
+        <v>16</v>
+      </c>
+      <c r="F639" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B640" t="s">
+        <v>21</v>
+      </c>
+      <c r="C640">
+        <v>4</v>
+      </c>
+      <c r="D640" t="s">
+        <v>22</v>
+      </c>
+      <c r="E640" t="s">
+        <v>16</v>
+      </c>
+      <c r="F640" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B641" t="s">
+        <v>621</v>
+      </c>
+      <c r="C641">
+        <v>9</v>
+      </c>
+      <c r="D641" t="s">
+        <v>622</v>
+      </c>
+      <c r="E641" t="s">
+        <v>16</v>
+      </c>
+      <c r="F641" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B642" t="s">
+        <v>49</v>
+      </c>
+      <c r="C642">
+        <v>2</v>
+      </c>
+      <c r="D642" t="s">
+        <v>50</v>
+      </c>
+      <c r="E642" t="s">
+        <v>16</v>
+      </c>
+      <c r="F642" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B643" t="s">
+        <v>876</v>
+      </c>
+      <c r="C643">
+        <v>2</v>
+      </c>
+      <c r="D643" t="s">
+        <v>877</v>
+      </c>
+      <c r="E643" t="s">
+        <v>16</v>
+      </c>
+      <c r="F643" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B644" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C644">
+        <v>1</v>
+      </c>
+      <c r="D644" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E644" t="s">
+        <v>16</v>
+      </c>
+      <c r="F644" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B645" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C645">
+        <v>3</v>
+      </c>
+      <c r="D645" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E645" t="s">
+        <v>16</v>
+      </c>
+      <c r="F645" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B646" t="s">
+        <v>216</v>
+      </c>
+      <c r="C646">
+        <v>12</v>
+      </c>
+      <c r="D646" t="s">
+        <v>217</v>
+      </c>
+      <c r="E646" t="s">
+        <v>16</v>
+      </c>
+      <c r="F646" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B647" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C647">
+        <v>1</v>
+      </c>
+      <c r="D647" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E647" t="s">
+        <v>16</v>
+      </c>
+      <c r="F647" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B648" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C648">
+        <v>1</v>
+      </c>
+      <c r="D648" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E648" t="s">
+        <v>16</v>
+      </c>
+      <c r="F648" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A649" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B649" t="s">
+        <v>424</v>
+      </c>
+      <c r="C649">
+        <v>8</v>
+      </c>
+      <c r="D649" t="s">
+        <v>425</v>
+      </c>
+      <c r="E649" t="s">
+        <v>16</v>
+      </c>
+      <c r="F649" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B650" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C650">
+        <v>1</v>
+      </c>
+      <c r="D650" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E650" t="s">
+        <v>16</v>
+      </c>
+      <c r="F650" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B651" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C651">
+        <v>1</v>
+      </c>
+      <c r="D651" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E651" t="s">
+        <v>16</v>
+      </c>
+      <c r="F651" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A652" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B652" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C652">
+        <v>1</v>
+      </c>
+      <c r="D652" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E652" t="s">
+        <v>16</v>
+      </c>
+      <c r="F652" t="s">
+        <v>1230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added july RMA details.
</commit_message>
<xml_diff>
--- a/Code/Failure_rate/2022/YTD_2022.xlsx
+++ b/Code/Failure_rate/2022/YTD_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\Failure_rate\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4CBCC-2C67-4625-BC5F-5FAE18011665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B093282F-8439-4D45-ABAB-E00C16700940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="23400" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="17730" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4875" uniqueCount="1741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="1975">
   <si>
     <t>RMA ID</t>
   </si>
@@ -5245,6 +5245,708 @@
   </si>
   <si>
     <t>RMA17138</t>
+  </si>
+  <si>
+    <t>RMA17158</t>
+  </si>
+  <si>
+    <t>RMA17212</t>
+  </si>
+  <si>
+    <t>RMA17207</t>
+  </si>
+  <si>
+    <t>RMA17189</t>
+  </si>
+  <si>
+    <t>RMA17163</t>
+  </si>
+  <si>
+    <t>RMA17156</t>
+  </si>
+  <si>
+    <t>RMA17165</t>
+  </si>
+  <si>
+    <t>SP-338-02-RD-F-L</t>
+  </si>
+  <si>
+    <t>3" MINI COMPLETE FT/FTIC ROUND FLANGED TO FLANGELESS</t>
+  </si>
+  <si>
+    <t>RMA17244</t>
+  </si>
+  <si>
+    <t>CMRD10-18CS1-5027KH-30-S-179-CR1-RM-MOD1</t>
+  </si>
+  <si>
+    <t>BEVELED MINI CYL RD DL 18W CSD RAL7047 49/72020 10" 5027KH 30° SOC CR1 RM MOD=CS+RM</t>
+  </si>
+  <si>
+    <t>RMA17243</t>
+  </si>
+  <si>
+    <t>MDF04-13H1-27KH-50-SM-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT FLANGE 4 CELL 13W 2700KH 50° SILVER MATTE-WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17171</t>
+  </si>
+  <si>
+    <t>CA2</t>
+  </si>
+  <si>
+    <t>TEE BAR ASM 24"- 30" CENTER CUT CEILING</t>
+  </si>
+  <si>
+    <t>RMA17183</t>
+  </si>
+  <si>
+    <t>CBRD10-24C3-35KS-50-S-WH-AJ3-UNV-D6E</t>
+  </si>
+  <si>
+    <t>2.2 CYLINDER RD DL 24W CW 3500KS 50° BEAM-SOLITE LENS-WHITE-AJ MOUNT 96" 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA17175</t>
+  </si>
+  <si>
+    <t>RMA17226</t>
+  </si>
+  <si>
+    <t>SP-324-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT DRIVER - REPLACEMENT MINI X FTA-0350mA 120V-277V DIML6E-TR</t>
+  </si>
+  <si>
+    <t>RMA17227</t>
+  </si>
+  <si>
+    <t>MDL08-27H1-30KH-50-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT TRIMLESS 8 CELL 27W 3000KH 50° WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17176</t>
+  </si>
+  <si>
+    <t>RMA17206</t>
+  </si>
+  <si>
+    <t>B4RART-33C3-35KS-T15-WH-RT-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD TRMD ADJ 33W 3500K 80CRI 15° BEAM RETROFIT WHITE HSG 120-277V ELDO 0-10V 1% LIN</t>
+  </si>
+  <si>
+    <t>RMA17152</t>
+  </si>
+  <si>
+    <t>RMA17181</t>
+  </si>
+  <si>
+    <t>RMA17209</t>
+  </si>
+  <si>
+    <t>RMA17245</t>
+  </si>
+  <si>
+    <t>RMA17191</t>
+  </si>
+  <si>
+    <t>RMA17202</t>
+  </si>
+  <si>
+    <t>MDG08-27H1-30KS-35-BL-BL-GL94-TRM</t>
+  </si>
+  <si>
+    <t>MICRO VS DOWNLIGHT 8 CELL 27W 3000KS 35° BLACK-BLACK GL94 TRIM</t>
+  </si>
+  <si>
+    <t>RMA17169</t>
+  </si>
+  <si>
+    <t>SR11-WH-X115-30KH-50-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>SLIVERLED RD DN 1" WHITE BFFL X115 3000KH-50°DISTRIBUTION-SOLITE CLEAR LENS-WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17153</t>
+  </si>
+  <si>
+    <t>RMA17211</t>
+  </si>
+  <si>
+    <t>CBRD10-36E1-35KS-50-S-BZ-PJ3-UNV-D6E</t>
+  </si>
+  <si>
+    <t>2.2 CYLINDER RD DL 36W CW 3500KS 50° BEAM-SOLITE LENS-BRONZE-PJ MOUNT 95" 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA17234</t>
+  </si>
+  <si>
+    <t>SP-189-0350-6B</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT SLIVERLED 350mA-DIML6B-EL</t>
+  </si>
+  <si>
+    <t>RMA17162</t>
+  </si>
+  <si>
+    <t>MDM04-13H1-30KS-35-BZ-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT MILLWORK 4 CELL 13W 3000K 80 CRI 35° BRONZE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17217</t>
+  </si>
+  <si>
+    <t>RMA17190</t>
+  </si>
+  <si>
+    <t>RMA17205</t>
+  </si>
+  <si>
+    <t>RPA-01-41H1-UNV-D8E-MOD1</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MICRO-1 FIXTURE MAX-41W H1 700mA 120-277V D8E-MOD=SINGLE FIXTURE</t>
+  </si>
+  <si>
+    <t>RMA17172</t>
+  </si>
+  <si>
+    <t>SP-126-0500-19</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT- BEVELED BASIC IC/CP HSG 20 WATT 500mA 120V-DIML19 HT</t>
+  </si>
+  <si>
+    <t>LEM-213-00-27KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BASIC BEVELED STD CRI 2700K</t>
+  </si>
+  <si>
+    <t>RMA17196</t>
+  </si>
+  <si>
+    <t>RMA17235</t>
+  </si>
+  <si>
+    <t>RMA17193</t>
+  </si>
+  <si>
+    <t>SP-140-0700-8</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - BEVELED 2.1 NC/IC/CP 16 WATT 700mA 120V-DIML8-EL</t>
+  </si>
+  <si>
+    <t>RMA17242</t>
+  </si>
+  <si>
+    <t>SP-322-0500-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT DRIVER-REPLACEMENT X1/X3/WG2/CS1 NC1/NCIC/NCCP-0500mA 120V-277V DIML6E-EL</t>
+  </si>
+  <si>
+    <t>RMA17216</t>
+  </si>
+  <si>
+    <t>RMA17221</t>
+  </si>
+  <si>
+    <t>RMA17213</t>
+  </si>
+  <si>
+    <t>RMA17177</t>
+  </si>
+  <si>
+    <t>RMA17198</t>
+  </si>
+  <si>
+    <t>RMA17186</t>
+  </si>
+  <si>
+    <t>SV-X115-IC-UNV-D6E</t>
+  </si>
+  <si>
+    <t>SLIVERLED SQ/RND TRIMMED 15W IC HSG 120-277V-DIML6E</t>
+  </si>
+  <si>
+    <t>SV-X109-IC-UNV-D6E</t>
+  </si>
+  <si>
+    <t>SLIVERLED SQ/RND TRIMMED 9W IC HSG UNV-DIML6E</t>
+  </si>
+  <si>
+    <t>RMA17240</t>
+  </si>
+  <si>
+    <t>RMA17173</t>
+  </si>
+  <si>
+    <t>RPB-01-18FC1-UNV-D23X2-RJ-MOD1</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI-18W INFINITE COLOR 350/350/350/700mA 120-277V 16BIT MAN-RJ45 JACKS-MOD=PRELIM</t>
+  </si>
+  <si>
+    <t>RMA17238</t>
+  </si>
+  <si>
+    <t>RMA17188</t>
+  </si>
+  <si>
+    <t>Z1RDF-07X4C-35KH-45-NC-RM-HSG</t>
+  </si>
+  <si>
+    <t>ZEPTO RD DL TRMD 07W CLASSIC 35K 90CRI 45° BEAM NC HSG REMOTE POWER SUPPLY</t>
+  </si>
+  <si>
+    <t>RMA17231</t>
+  </si>
+  <si>
+    <t>MDG02-08H1-NCVS-UNV-D6E-GL94-HSG</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 2 CELL 8W NCVS UNV ELDOLED 0-10V 1% LIN GL94 HSG</t>
+  </si>
+  <si>
+    <t>UA2</t>
+  </si>
+  <si>
+    <t>GRID MOUNT BAR SET 16-24"</t>
+  </si>
+  <si>
+    <t>RMA17222</t>
+  </si>
+  <si>
+    <t>MDG02-08H1-30KS-50-BL-BL-GL94-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 2 CELL 8W 3000K 80 CRI 50° BLACK-BLACK GL94 TRIM</t>
+  </si>
+  <si>
+    <t>MWL02-08H1-30KH-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO WW TRIMLESS 2 CELL 8W 3000KH WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17232</t>
+  </si>
+  <si>
+    <t>RMA17210</t>
+  </si>
+  <si>
+    <t>SP-420-0350-2</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENTMINI PRIMARY EC 15W 350mA D2</t>
+  </si>
+  <si>
+    <t>RMA17159</t>
+  </si>
+  <si>
+    <t>M1RAF-07X4C-30KH-50-M0-WH-WH-RT-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD ADJ TRMD 7W 3000K 90 CRI 50° BEAM MICRO DIF LENS WHITE WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17155</t>
+  </si>
+  <si>
+    <t>CK27</t>
+  </si>
+  <si>
+    <t>27" C-CHANNEL BARS/BUTTER FLY BRACKETS</t>
+  </si>
+  <si>
+    <t>P4RDF-22L2-40KS-F-NC-UNV-D22-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 PRIMARY RD DL TRMD 22W L2 40K 80CRI FLOOD OPTIC 120-277V D22 NC HSG</t>
+  </si>
+  <si>
+    <t>RMA17230</t>
+  </si>
+  <si>
+    <t>MDG02-08H1-30KH-35-BL-BL-GL91-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 2 CELL 8W 3000K 90 CRI 35° BLACK-BLACK GL91 TRIM</t>
+  </si>
+  <si>
+    <t>RMA17166</t>
+  </si>
+  <si>
+    <t>SAMPLE BOX LITTLEONES MICRO KRAFT</t>
+  </si>
+  <si>
+    <t>RMA17195</t>
+  </si>
+  <si>
+    <t>SP-324-0350-28</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT DRIVER-REPLACEMENT MINI X FTA-350mA 120V-277V DIML28-EL</t>
+  </si>
+  <si>
+    <t>RMA17174</t>
+  </si>
+  <si>
+    <t>RMA17224</t>
+  </si>
+  <si>
+    <t>RMA17215</t>
+  </si>
+  <si>
+    <t>RPB-01-20M2-UNV-D6F</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX-20W M2 500mA 120-277V D6F</t>
+  </si>
+  <si>
+    <t>SP-087-1400-6F</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-BEVELED 6" PENDANT-33W-1400mA-120V-277V DIML6F-EL</t>
+  </si>
+  <si>
+    <t>RMA17236</t>
+  </si>
+  <si>
+    <t>SP-317-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.2 NC HSG 9W 350mA 120V-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA17218</t>
+  </si>
+  <si>
+    <t>B3RGF-15X3-30KH-30-NCIC-120V-D22-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRMD 15W 3000K 90 CRI 30° BEAM SLOPED  HSG 120V ERP 0-10V, 1%</t>
+  </si>
+  <si>
+    <t>RMA17167</t>
+  </si>
+  <si>
+    <t>B3RGF-30-S-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL TRMD 30° SLOPED SOLITE CLEAR LENS WHITE BEVEL WHITE FLANGE</t>
+  </si>
+  <si>
+    <t>RMA17208</t>
+  </si>
+  <si>
+    <t>RMA17197</t>
+  </si>
+  <si>
+    <t>RMA17201</t>
+  </si>
+  <si>
+    <t>RMA17161</t>
+  </si>
+  <si>
+    <t>RPD-01-09X1M-UNV-D6B</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER LITTLEONES-1 FIXTURE/DRIVER-9W X1M 225mA 120-277V D6B</t>
+  </si>
+  <si>
+    <t>M1RDF-09X1M-NC-RM-HSG</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRMD 9W NC RM HSG</t>
+  </si>
+  <si>
+    <t>RMA17192</t>
+  </si>
+  <si>
+    <t>RPB-01-20WG2-UNV-D6E</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX-20W WG2 500mA 120-277V D6E</t>
+  </si>
+  <si>
+    <t>LEM-313-00-2722KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BEVELED MINI WGD HI CRI 2700-2200KH</t>
+  </si>
+  <si>
+    <t>RMA17184</t>
+  </si>
+  <si>
+    <t>LEM-275-16-2722KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 WG2 16W 80CRI 2700-2200K</t>
+  </si>
+  <si>
+    <t>RMA17200</t>
+  </si>
+  <si>
+    <t>RMA17157</t>
+  </si>
+  <si>
+    <t>USAI-4DLA1IC-FC1IX32D23-RPG-00</t>
+  </si>
+  <si>
+    <t>RECESS 4.5 RD ADJ TRML 32W INFINITE COLOR+ 40° BEAM NCIC HSG 120-277V DMX 0.1% DIM RJ45</t>
+  </si>
+  <si>
+    <t>USAI-4DLA1IC-FC1IX32D23-RPF-00</t>
+  </si>
+  <si>
+    <t>RECESS 4.5 RD ADJ TRML 32W INFINITE COLOR+ 35° BEAM NCIC HSG 120-277V DMX 0.1% DIM RJ45</t>
+  </si>
+  <si>
+    <t>RMA17204</t>
+  </si>
+  <si>
+    <t>SP-457-0700-23X1</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT- BEVELED 2.2 CYLINDER 32W FC1 120-277V D23X1 8 BIT MANUAL ADDRESS</t>
+  </si>
+  <si>
+    <t>RMA17223</t>
+  </si>
+  <si>
+    <t>USAI-4DLA1NC-FC1IX32D23-RFF-00</t>
+  </si>
+  <si>
+    <t>RECESS 4.5 RD ADJ TRMD 32W INFINITE COLOR+ 35° BEAM NC HSG 120-277V DMX 0.1% DIM RJ45</t>
+  </si>
+  <si>
+    <t>RMA17187</t>
+  </si>
+  <si>
+    <t>USAI-2DL-WGD-IP-CONTROLLER-00</t>
+  </si>
+  <si>
+    <t>REPLACEMENT CONTROLLER PLATE ASSY - 0500 WGD MINI NC1 W/ PLATE</t>
+  </si>
+  <si>
+    <t>USAI-2DL-DRIVER-NC-WD1IP16A-00</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT PINHOLE 700mA-D3 WGD</t>
+  </si>
+  <si>
+    <t>RMA17239</t>
+  </si>
+  <si>
+    <t>B4SDF-S-SC-SC-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED SQUARE TRMD DL/ADJ SOLITE LENS CONDUIT SILVER TRIM</t>
+  </si>
+  <si>
+    <t>B4SDF-12C3-35KS-90-NCSM-UNV-D7-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 SQ DL TRMD 12W CLASSIC 35K 80CRI 90° BEAM NCSM HSG 120-277V ELDO DALI 0.1% DIM</t>
+  </si>
+  <si>
+    <t>RMA17228</t>
+  </si>
+  <si>
+    <t>RMA17194</t>
+  </si>
+  <si>
+    <t>B3RCL-15WG2-2722KH-30-NC1-UNV-D6A-HSG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEVELED MINI RD COMFORT TRML 15W WARM GLOW 27-22K 90CRI 30° BEAM NC1 HSG 120-277V D6A </t>
+  </si>
+  <si>
+    <t>B4RAL-32WG2-2722KH-R40-NC-UNV-D6A-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD ADJ TRML 32W WARM GLOW 27-22K 90CRI 40° BEAM NC HSG 120-277V ELDO 0.1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA17203</t>
+  </si>
+  <si>
+    <t>B4RCL-32WG2-2722KH-65-NC-UNV-D6A-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD COMFORT TRML 32W WARM GLOW 27-22K 90CRI 65° BEAM NC HSG 120-277V ELDO 0.1% LIN DIM</t>
+  </si>
+  <si>
+    <t>B3RAF-15WG2-2722KH-30-NC1-UNV-D6A-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD ADJ TRMD 15W WARM GLOW 27-22K 90CRI 30° BEAM NC1 HSG 120-277V D6A</t>
+  </si>
+  <si>
+    <t>RMA17225</t>
+  </si>
+  <si>
+    <t>P3SF-15L2-EC-UNV-D22-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI PRIMARY SQUARE TRMD 15W L2 120-277V D22 EC HSG</t>
+  </si>
+  <si>
+    <t>B4RAL-32WG2-2722KH-T62-NC-UNV-D6A-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD ADJ TRML 32W WARM GLOW 27-22K 90CRI 20°x60°BEAM NC HSG 120-277V ELDO 0.1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA17233</t>
+  </si>
+  <si>
+    <t>RMA17214</t>
+  </si>
+  <si>
+    <t>SP-534-0350-22</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - PRIMARY NXT 15W D22</t>
+  </si>
+  <si>
+    <t>RMA17237</t>
+  </si>
+  <si>
+    <t>B3RAF-25-S-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI ROUND DL/ADJ TRMD 0°-40° TILT SOLITE LENS -WHITE BEVEL-WHITE FLANGE TRIM</t>
+  </si>
+  <si>
+    <t>B3RAF-15L2-27KS-25-NC-UNV-D22-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD ADJ TRMD 15W BASIC 27K 80CRI 25° BEAM NC HSG 120-277V D22</t>
+  </si>
+  <si>
+    <t>RMA17151</t>
+  </si>
+  <si>
+    <t>RMA17154</t>
+  </si>
+  <si>
+    <t>M1RDL-07X4C-27KH-35-M0-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRML 7W 2700K 90 CRI 35° BEAM MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>M1RDL-09X1M-27KH-35-M0-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRML 9W 2700K 90 CRI 35° BEAM MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17220</t>
+  </si>
+  <si>
+    <t>B3SWL-18FC1-W3-NC1-UNV-RM-HSG-MOD1</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ WW3 TRML 18W INFINITE COLOR 30K 80CRI NC1 HSG D23 MOD=W3</t>
+  </si>
+  <si>
+    <t>B3RWP-18CS1-6022KS-W2-NC1-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD WW TRML TILE 18W COLOR SELECT 60-22K 80CRI NC1 HSG 120-277V D6E</t>
+  </si>
+  <si>
+    <t>B3RCP-18CS1-6022KS-50-NC1-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD COMFORT TRML TILE 18W COLOR SELECT 60-22K 80CRI 50° BEAM NC1 HSG 120-277V D6E</t>
+  </si>
+  <si>
+    <t>B3SCP-18FC1-45-NC1-UNV-D23X1-WR-HSG-MOD1</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ COMFORT TRML TILE 18W INFINITE COLOR 30K 80CRI 45° BEAM NC1 HSG  D23 MOD = NS ABOVE</t>
+  </si>
+  <si>
+    <t>B3SCP-18FC1-55-NC1-RM-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ COMFORT TRML TILE 18W INFINITE COLOR 30K 80CRI 55° BEAM NC1 HSG RM</t>
+  </si>
+  <si>
+    <t>B3RAP-18FC1-35-NC1-UNV-D23X1-WR-HSG-MOD1</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD WW MILLWORK WH 18W INFINITE COLOR 30K 80CRI NC1 HSG D23 MOD = NS ABOVE CEILING</t>
+  </si>
+  <si>
+    <t>B3SDL-18FC1-65-FT-RM-HSG-MOD1</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ DL TRML 18W INFINITE COLOR 30K 80CRI 65° BEAM FT HSG  REMOTE DRIVER-MOD=PRELIM</t>
+  </si>
+  <si>
+    <t>B3RAP-18CS1-6022KS-30-NC1-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD ADJ TRML TILE 18W COLOR SELECT 60-22K 80CRI 30° BEAM NC1 HSG 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA17164</t>
+  </si>
+  <si>
+    <t>SP-421-0350-21</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - PRIMARY BEVEL ADJ NC/IC HSG</t>
+  </si>
+  <si>
+    <t>LEM-401-00-3018KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT PRIMARY HI CRI 3000K-1800K</t>
+  </si>
+  <si>
+    <t>RMA17241</t>
+  </si>
+  <si>
+    <t>M1SWL-07X4C-30KS-W2-D1-WH-IC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO SQ WW TRML 7W 3000K 80 CRI W2 MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA17180</t>
+  </si>
+  <si>
+    <t>RMA17199</t>
+  </si>
+  <si>
+    <t>AC3951-118-B1-1196</t>
+  </si>
+  <si>
+    <t>BEVELED CUSTOM ROUND WW 118.5 DIA FLANGE APPLE MARRONE BRONZO</t>
+  </si>
+  <si>
+    <t>July</t>
   </si>
 </sst>
 </file>
@@ -5635,11 +6337,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F975"/>
+  <dimension ref="A1:F1110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A968" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L811" sqref="L811"/>
+      <pane ySplit="1" topLeftCell="A1094" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1116" sqref="F1116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25144,6 +25846,2700 @@
         <v>1510</v>
       </c>
     </row>
+    <row r="976" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A976" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B976" t="s">
+        <v>691</v>
+      </c>
+      <c r="C976">
+        <v>1</v>
+      </c>
+      <c r="D976" t="s">
+        <v>692</v>
+      </c>
+      <c r="E976" t="s">
+        <v>16</v>
+      </c>
+      <c r="F976" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="977" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A977" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B977" t="s">
+        <v>151</v>
+      </c>
+      <c r="C977">
+        <v>11</v>
+      </c>
+      <c r="D977" t="s">
+        <v>152</v>
+      </c>
+      <c r="E977" t="s">
+        <v>16</v>
+      </c>
+      <c r="F977" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="978" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A978" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B978" t="s">
+        <v>37</v>
+      </c>
+      <c r="C978">
+        <v>4</v>
+      </c>
+      <c r="D978" t="s">
+        <v>38</v>
+      </c>
+      <c r="E978" t="s">
+        <v>16</v>
+      </c>
+      <c r="F978" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="979" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B979" t="s">
+        <v>41</v>
+      </c>
+      <c r="C979">
+        <v>1</v>
+      </c>
+      <c r="D979" t="s">
+        <v>42</v>
+      </c>
+      <c r="E979" t="s">
+        <v>16</v>
+      </c>
+      <c r="F979" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="980" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B980" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C980">
+        <v>1</v>
+      </c>
+      <c r="D980" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E980" t="s">
+        <v>16</v>
+      </c>
+      <c r="F980" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="981" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B981" t="s">
+        <v>240</v>
+      </c>
+      <c r="C981">
+        <v>1</v>
+      </c>
+      <c r="D981" t="s">
+        <v>241</v>
+      </c>
+      <c r="E981" t="s">
+        <v>9</v>
+      </c>
+      <c r="F981" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="982" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B982" t="s">
+        <v>240</v>
+      </c>
+      <c r="C982">
+        <v>4</v>
+      </c>
+      <c r="D982" t="s">
+        <v>241</v>
+      </c>
+      <c r="E982" t="s">
+        <v>16</v>
+      </c>
+      <c r="F982" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="983" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B983" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C983">
+        <v>11</v>
+      </c>
+      <c r="D983" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E983" t="s">
+        <v>127</v>
+      </c>
+      <c r="F983" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="984" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B984" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C984">
+        <v>223</v>
+      </c>
+      <c r="D984" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E984" t="s">
+        <v>127</v>
+      </c>
+      <c r="F984" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="985" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B985" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C985">
+        <v>1</v>
+      </c>
+      <c r="D985" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E985" t="s">
+        <v>16</v>
+      </c>
+      <c r="F985" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="986" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B986" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C986">
+        <v>153</v>
+      </c>
+      <c r="D986" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E986" t="s">
+        <v>127</v>
+      </c>
+      <c r="F986" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="987" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B987" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C987">
+        <v>28</v>
+      </c>
+      <c r="D987" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E987" t="s">
+        <v>9</v>
+      </c>
+      <c r="F987" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="988" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B988" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C988">
+        <v>2</v>
+      </c>
+      <c r="D988" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E988" t="s">
+        <v>9</v>
+      </c>
+      <c r="F988" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="989" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B989" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C989">
+        <v>1</v>
+      </c>
+      <c r="D989" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E989" t="s">
+        <v>16</v>
+      </c>
+      <c r="F989" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="990" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B990" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C990">
+        <v>1</v>
+      </c>
+      <c r="D990" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E990" t="s">
+        <v>16</v>
+      </c>
+      <c r="F990" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="991" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B991" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C991">
+        <v>1</v>
+      </c>
+      <c r="D991" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E991" t="s">
+        <v>16</v>
+      </c>
+      <c r="F991" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="992" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B992" t="s">
+        <v>167</v>
+      </c>
+      <c r="C992">
+        <v>6</v>
+      </c>
+      <c r="D992" t="s">
+        <v>168</v>
+      </c>
+      <c r="E992" t="s">
+        <v>16</v>
+      </c>
+      <c r="F992" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="993" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A993" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B993" t="s">
+        <v>21</v>
+      </c>
+      <c r="C993">
+        <v>13</v>
+      </c>
+      <c r="D993" t="s">
+        <v>22</v>
+      </c>
+      <c r="E993" t="s">
+        <v>16</v>
+      </c>
+      <c r="F993" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="994" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A994" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B994" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C994">
+        <v>1</v>
+      </c>
+      <c r="D994" t="s">
+        <v>1772</v>
+      </c>
+      <c r="E994" t="s">
+        <v>127</v>
+      </c>
+      <c r="F994" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="995" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A995" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B995" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C995">
+        <v>1</v>
+      </c>
+      <c r="D995" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E995" t="s">
+        <v>9</v>
+      </c>
+      <c r="F995" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="996" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A996" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B996" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C996">
+        <v>3</v>
+      </c>
+      <c r="D996" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E996" t="s">
+        <v>9</v>
+      </c>
+      <c r="F996" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="997" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B997" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C997">
+        <v>57</v>
+      </c>
+      <c r="D997" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E997" t="s">
+        <v>127</v>
+      </c>
+      <c r="F997" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="998" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B998" t="s">
+        <v>885</v>
+      </c>
+      <c r="C998">
+        <v>1</v>
+      </c>
+      <c r="D998" t="s">
+        <v>886</v>
+      </c>
+      <c r="E998" t="s">
+        <v>16</v>
+      </c>
+      <c r="F998" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="999" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A999" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B999" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C999">
+        <v>1</v>
+      </c>
+      <c r="D999" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E999" t="s">
+        <v>16</v>
+      </c>
+      <c r="F999" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1000" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>734</v>
+      </c>
+      <c r="C1000">
+        <v>3</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1001" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1001">
+        <v>10</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1002" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C1002">
+        <v>1</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1003" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C1003">
+        <v>1</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1004" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>711</v>
+      </c>
+      <c r="C1004">
+        <v>4</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>712</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1005" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C1005">
+        <v>4</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1006" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C1006">
+        <v>1</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1007" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C1007">
+        <v>1</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1008" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1008">
+        <v>1</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1009" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>691</v>
+      </c>
+      <c r="C1009">
+        <v>1</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>692</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1010" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C1010">
+        <v>17</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1011" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1011">
+        <v>26</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>1801</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1012" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1012">
+        <v>26</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1013" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1013">
+        <v>4</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1014" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C1014">
+        <v>3</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1014" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1015" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1015">
+        <v>3</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1015" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1016" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C1016">
+        <v>1</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1016" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1017" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C1017">
+        <v>1</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>1811</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1017" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1018" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1018">
+        <v>10</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>989</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1019" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1019">
+        <v>2</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1020" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C1020">
+        <v>5</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>1652</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1020" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1021" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1021">
+        <v>1</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1021" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1022" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C1022">
+        <v>24</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1022" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1023" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1023">
+        <v>63</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1023" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1024" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1024">
+        <v>6</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1024" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1025" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1025">
+        <v>4</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1025" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1026" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1026">
+        <v>61</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1026" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1027" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1027">
+        <v>1</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1027" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1028" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1028">
+        <v>7</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1028" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1029" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1029">
+        <v>14</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1029" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1030" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1030">
+        <v>15</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1030" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1031" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1031">
+        <v>2</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1031" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1032" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1032">
+        <v>16</v>
+      </c>
+      <c r="D1032" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1032" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1033" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1033">
+        <v>9</v>
+      </c>
+      <c r="D1033" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1033" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1034" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>621</v>
+      </c>
+      <c r="C1034">
+        <v>9</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>622</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1035" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1035">
+        <v>2</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1035" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1036" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C1036">
+        <v>1</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1036" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1037" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C1037">
+        <v>1</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>1829</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1037" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1038" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C1038">
+        <v>10</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>1832</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1038" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1039" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C1039">
+        <v>10</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>1834</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1040" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>667</v>
+      </c>
+      <c r="C1040">
+        <v>1</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>668</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1041" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1041">
+        <v>10</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>1837</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1042" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1042">
+        <v>2</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1042" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1043" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>667</v>
+      </c>
+      <c r="C1043">
+        <v>1</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>668</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1044" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1044">
+        <v>1</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>1843</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1044" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1045" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1045">
+        <v>15</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1045" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1046" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1046">
+        <v>10</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1047" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C1047">
+        <v>5</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F1047" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1048" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1048">
+        <v>5</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>533</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1048" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1049" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C1049">
+        <v>5</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F1049" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1050" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C1050">
+        <v>2</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>1854</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1050" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1051" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C1051">
+        <v>1</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>1856</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1051" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1052" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C1052">
+        <v>2</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>1859</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1052" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1053" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1053">
+        <v>6</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1053" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1054" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1054">
+        <v>1</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>432</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1055" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>667</v>
+      </c>
+      <c r="C1055">
+        <v>1</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>668</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1056" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C1056">
+        <v>2</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>1864</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1057">
+        <v>25</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1058">
+        <v>2</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1059" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C1059">
+        <v>25</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>1866</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1060" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C1060">
+        <v>5</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>1869</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1061" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C1061">
+        <v>4</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>1872</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1062" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C1062">
+        <v>8</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>1875</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1063" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1063">
+        <v>4</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1064" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1064">
+        <v>1</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1065" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C1065">
+        <v>1</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1066" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C1066">
+        <v>5</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>1881</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1067" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C1067">
+        <v>2</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>1883</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1068" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>1885</v>
+      </c>
+      <c r="C1068">
+        <v>1</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>1886</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1069" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1887</v>
+      </c>
+      <c r="C1069">
+        <v>1</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>1888</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1070" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C1070">
+        <v>9</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>1891</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1071" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1071">
+        <v>16</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1071" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1072" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C1072">
+        <v>3</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>1895</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1072" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1073" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C1073">
+        <v>12</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1073" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1074" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C1074">
+        <v>1</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>1900</v>
+      </c>
+      <c r="E1074" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1074" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1075" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C1075">
+        <v>2</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>1903</v>
+      </c>
+      <c r="E1075" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1075" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1076" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C1076">
+        <v>1</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E1076" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1076" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1077" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C1077">
+        <v>1</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>1908</v>
+      </c>
+      <c r="E1077" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1077" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1078" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>343</v>
+      </c>
+      <c r="C1078">
+        <v>1</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1078" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1079" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C1079">
+        <v>1</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E1079" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1079" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1080" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C1080">
+        <v>1</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>1913</v>
+      </c>
+      <c r="E1080" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1080" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1081" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1081">
+        <v>10</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1081" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1082" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C1082">
+        <v>14</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>1917</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1082" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1083" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C1083">
+        <v>45</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>1917</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1083" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1084" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C1084">
+        <v>17</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>1919</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1084" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1085" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1085">
+        <v>3</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1085" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1086" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C1086">
+        <v>42</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>1922</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1086" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1087" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C1087">
+        <v>5</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>1924</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1087" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1088" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C1088">
+        <v>6</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>1927</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1088" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1089" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C1089">
+        <v>17</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1089" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1090" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>725</v>
+      </c>
+      <c r="C1090">
+        <v>1</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>726</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1091" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C1091">
+        <v>22</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1091" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1092" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C1092">
+        <v>6</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>1936</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1092" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1093" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C1093">
+        <v>6</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1093" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1094" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>343</v>
+      </c>
+      <c r="C1094">
+        <v>6</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1094" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1095" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1095">
+        <v>17</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1096" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C1096">
+        <v>3</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>1942</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1097" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C1097">
+        <v>1</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>1944</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1098" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C1098">
+        <v>8</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>1947</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1099" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C1099">
+        <v>5</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>1949</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1099" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1100" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C1100">
+        <v>1</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>1951</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1100" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1101" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C1101">
+        <v>5</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>1953</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1101" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1102" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C1102">
+        <v>2</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>1955</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>1956</v>
+      </c>
+      <c r="C1103">
+        <v>7</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>1957</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1103" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1104" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C1104">
+        <v>3</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>1959</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1104" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1105" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C1105">
+        <v>2</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>1961</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1105" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1106" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C1106">
+        <v>1</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>1964</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1107" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C1107">
+        <v>1</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1108" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C1108">
+        <v>1</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1108" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1109" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>688</v>
+      </c>
+      <c r="C1109">
+        <v>1</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>689</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1109" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C1110">
+        <v>43</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>1973</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1110" t="s">
+        <v>1974</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>